<commit_message>
-Ema's Supercomputer- Challenge with progress, at 34% Efficacy, need a plus overlap check aux function to finish
</commit_message>
<xml_diff>
--- a/HackerRank/Problem Solving/Observations/Challenges Observations.xlsx
+++ b/HackerRank/Problem Solving/Observations/Challenges Observations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\GR\Software Development\Learning\HackerRank\Problem Solving\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569ACF8A-C46A-4C56-98D4-87A66B71E679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B35EE1-61D2-4740-89A0-672FF8D91926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="807" activeTab="4" xr2:uid="{02547566-692A-4121-816D-BFBD3A86BC7B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="32">
   <si>
     <t>If qPos</t>
   </si>
@@ -125,6 +125,18 @@
   <si>
     <t>['BGBBBBB','GGGBBBB','BGBBGBB','BBBBGBB','BBGGGGG','BBBBGBB','BBBBGBB']</t>
   </si>
+  <si>
+    <t>['BBBGBBBBBB','BBBGBBBBBB','BBBGBBBBBB','GGGGGGGBBB','BBBGBBGBBB','BBBGBBGBBB','BBBGGGGGGB','BBBBBBGBBB','BBBBBBGBBB','BBBBBBBBBB']</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>13 x 9</t>
+  </si>
+  <si>
+    <t>5 x 9</t>
+  </si>
 </sst>
 </file>
 
@@ -168,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,8 +319,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -476,11 +494,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,7 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -695,13 +801,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -725,11 +828,63 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -7611,287 +7766,2541 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCDF995-7901-458F-928B-4A20B2B19B7F}">
-  <dimension ref="F3:Q21"/>
+  <dimension ref="I3:AJ80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="G55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA74" sqref="AA74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="2.6640625" customWidth="1"/>
-    <col min="13" max="15" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="34" width="2.6640625" customWidth="1"/>
+    <col min="35" max="35" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-    </row>
-    <row r="4" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="L4" s="27"/>
-    </row>
-    <row r="5" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F5" s="25"/>
-      <c r="I5" s="28"/>
-      <c r="L5" s="27"/>
-      <c r="N5">
+    <row r="3" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="24"/>
+    </row>
+    <row r="4" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P4" s="25"/>
+      <c r="S4" s="26"/>
+      <c r="V4" s="27"/>
+    </row>
+    <row r="5" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P5" s="25"/>
+      <c r="S5" s="28"/>
+      <c r="V5" s="27"/>
+      <c r="AG5">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
-      <c r="M6">
+    <row r="6" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="27"/>
+      <c r="AF6">
         <v>3.2</v>
       </c>
-      <c r="O6">
+      <c r="AH6">
         <v>3.4</v>
       </c>
     </row>
-    <row r="7" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F7" s="25"/>
-      <c r="I7" s="28"/>
-      <c r="L7" s="27"/>
-      <c r="N7">
+    <row r="7" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P7" s="25"/>
+      <c r="S7" s="28"/>
+      <c r="V7" s="27"/>
+      <c r="AG7">
         <v>4.3</v>
       </c>
     </row>
-    <row r="8" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F8" s="25"/>
-      <c r="I8" s="26"/>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
-    </row>
-    <row r="13" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="P13" t="s">
+    <row r="8" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P8" s="25"/>
+      <c r="S8" s="26"/>
+      <c r="V8" s="27"/>
+    </row>
+    <row r="9" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="32"/>
+    </row>
+    <row r="13" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="AI13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F15" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="76"/>
-      <c r="P15" t="str">
-        <f>+_xlfn.CONCAT("'",F15:L15,"'")</f>
+    <row r="15" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P15" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="R15" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="S15" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="U15" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="V15" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI15" t="str">
+        <f>+_xlfn.CONCAT("'",P15:V15,"'")</f>
         <v>'BGBBBBB'</v>
       </c>
-      <c r="Q15" t="str">
-        <f>+_xlfn.CONCAT("[",P15,",",P16,",",P17,",",P18,",",P19,",",P20,",",P21,"]")</f>
+      <c r="AJ15" t="str">
+        <f>+_xlfn.CONCAT("[",AI15,",",AI16,",",AI17,",",AI18,",",AI19,",",AI20,",",AI21,"]")</f>
         <v>['BGBBBBB','GGGBBBB','BGBBGBB','BBBBGBB','BBGGGGG','BBBBGBB','BBBBGBB']</v>
       </c>
     </row>
-    <row r="16" spans="6:17" x14ac:dyDescent="0.3">
-      <c r="F16" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="76"/>
-      <c r="P16" t="str">
-        <f t="shared" ref="P16:P21" si="0">+_xlfn.CONCAT("'",F16:L16,"'")</f>
+    <row r="16" spans="16:36" x14ac:dyDescent="0.3">
+      <c r="P16" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q16" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="R16" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S16" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U16" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V16" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI16" t="str">
+        <f t="shared" ref="AI16:AI21" si="0">+_xlfn.CONCAT("'",P16:V16,"'")</f>
         <v>'GGGBBBB'</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="AJ16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F17" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="L17" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" s="76"/>
-      <c r="P17" t="str">
+    <row r="17" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="P17" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="S17" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="U17" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V17" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI17" t="str">
         <f t="shared" si="0"/>
         <v>'BGBBGBB'</v>
       </c>
     </row>
-    <row r="18" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F18" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" s="76"/>
-      <c r="P18" t="str">
+    <row r="18" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="P18" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R18" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="S18" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T18" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="U18" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V18" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI18" t="str">
         <f t="shared" si="0"/>
         <v>'BBBBGBB'</v>
       </c>
     </row>
-    <row r="19" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F19" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="76"/>
-      <c r="P19" t="str">
+    <row r="19" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="P19" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R19" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="T19" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="U19" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="V19" s="85" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI19" t="str">
         <f t="shared" si="0"/>
         <v>'BBGGGGG'</v>
       </c>
     </row>
-    <row r="20" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F20" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="85" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="76"/>
-      <c r="P20" t="str">
+    <row r="20" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="P20" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q20" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R20" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="S20" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T20" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="U20" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V20" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI20" t="str">
         <f t="shared" si="0"/>
         <v>'BBBBGBB'</v>
       </c>
     </row>
-    <row r="21" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F21" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="90" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21" s="89" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="76"/>
-      <c r="P21" t="str">
+    <row r="21" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="P21" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="U21" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="V21" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI21" t="str">
         <f t="shared" si="0"/>
         <v>'BBBBGBB'</v>
       </c>
     </row>
+    <row r="23" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI24" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ24" s="95">
+        <f>5*9</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="90"/>
+      <c r="S25" s="90"/>
+      <c r="T25" s="90"/>
+      <c r="U25" s="90"/>
+      <c r="V25" s="90"/>
+      <c r="W25" s="90"/>
+      <c r="X25" s="90"/>
+      <c r="Y25" s="90"/>
+      <c r="Z25" s="90"/>
+      <c r="AA25" s="90"/>
+      <c r="AB25" s="90"/>
+    </row>
+    <row r="26" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="90"/>
+      <c r="Q26" s="90"/>
+      <c r="R26" s="90"/>
+      <c r="S26" s="90"/>
+      <c r="T26" s="90"/>
+      <c r="U26" s="90"/>
+      <c r="V26" s="90"/>
+      <c r="W26" s="90"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="90"/>
+      <c r="Z26" s="90"/>
+      <c r="AA26" s="90"/>
+      <c r="AB26" s="90"/>
+    </row>
+    <row r="27" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="90"/>
+      <c r="Q27" s="90"/>
+      <c r="R27" s="90"/>
+      <c r="S27" s="90"/>
+      <c r="T27" s="90"/>
+      <c r="U27" s="90"/>
+      <c r="V27" s="90"/>
+      <c r="W27" s="90"/>
+      <c r="X27" s="90"/>
+      <c r="Y27" s="90"/>
+      <c r="Z27" s="90"/>
+      <c r="AA27" s="90"/>
+      <c r="AB27" s="90"/>
+    </row>
+    <row r="28" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="90"/>
+      <c r="Q28" s="90"/>
+      <c r="R28" s="90"/>
+      <c r="S28" s="90"/>
+      <c r="T28" s="90"/>
+      <c r="U28" s="90"/>
+      <c r="V28" s="90"/>
+      <c r="W28" s="90"/>
+      <c r="X28" s="90"/>
+      <c r="Y28" s="90"/>
+      <c r="Z28" s="90"/>
+      <c r="AA28" s="90"/>
+      <c r="AB28" s="90"/>
+      <c r="AI28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="90"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="90"/>
+      <c r="S29" s="90"/>
+      <c r="T29" s="90"/>
+      <c r="U29" s="90"/>
+      <c r="V29" s="90"/>
+      <c r="W29" s="90"/>
+      <c r="X29" s="90"/>
+      <c r="Y29" s="90"/>
+      <c r="Z29" s="90"/>
+      <c r="AA29" s="90"/>
+      <c r="AB29" s="90"/>
+    </row>
+    <row r="30" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="P30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="R30" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="S30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="T30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="U30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="V30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="W30" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="X30" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y30" s="90"/>
+      <c r="Z30" s="90"/>
+      <c r="AA30" s="90"/>
+      <c r="AB30" s="90"/>
+      <c r="AI30" t="str">
+        <f>+_xlfn.CONCAT("'",O30:X30,"'")</f>
+        <v>'BBBGBBBBBB'</v>
+      </c>
+      <c r="AJ30" t="str">
+        <f>+_xlfn.CONCAT("[",AI30,",",AI31,",",AI32,",",AI33,",",AI34,",",AI35,",",AI36,",",AI37,",",AI38,",",AI39,"]")</f>
+        <v>['BBBGBBBBBB','BBBGBBBBBB','BBBGBBBBBB','GGGGGGGBBB','BBBGBBGBBB','BBBGBBGBBB','BBBGGGGGGB','BBBBBBGBBB','BBBBBBGBBB','BBBBBBBBBB']</v>
+      </c>
+    </row>
+    <row r="31" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I31" s="90"/>
+      <c r="J31" s="90"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="90"/>
+      <c r="N31" s="90"/>
+      <c r="O31" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R31" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="T31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="U31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="V31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W31" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X31" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y31" s="90"/>
+      <c r="Z31" s="90"/>
+      <c r="AA31" s="90"/>
+      <c r="AB31" s="90"/>
+      <c r="AI31" t="str">
+        <f t="shared" ref="AI31:AI39" si="1">+_xlfn.CONCAT("'",O31:X31,"'")</f>
+        <v>'BBBGBBBBBB'</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="90"/>
+      <c r="N32" s="90"/>
+      <c r="O32" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="T32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="U32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="V32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W32" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X32" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y32" s="90"/>
+      <c r="Z32" s="90"/>
+      <c r="AA32" s="90"/>
+      <c r="AB32" s="90"/>
+      <c r="AI32" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBGBBBBBB'</v>
+      </c>
+    </row>
+    <row r="33" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="90"/>
+      <c r="N33" s="90"/>
+      <c r="O33" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="P33" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q33" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R33" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="S33" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T33" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V33" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W33" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X33" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y33" s="90"/>
+      <c r="Z33" s="90"/>
+      <c r="AA33" s="90"/>
+      <c r="AB33" s="90"/>
+      <c r="AI33" t="str">
+        <f t="shared" si="1"/>
+        <v>'GGGGGGGBBB'</v>
+      </c>
+    </row>
+    <row r="34" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q34" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R34" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S34" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="T34" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="U34" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V34" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W34" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X34" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y34" s="90"/>
+      <c r="Z34" s="90"/>
+      <c r="AA34" s="90"/>
+      <c r="AB34" s="90"/>
+      <c r="AI34" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBGBBGBBB'</v>
+      </c>
+    </row>
+    <row r="35" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P35" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q35" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R35" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S35" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="T35" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="U35" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V35" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W35" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X35" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y35" s="90"/>
+      <c r="Z35" s="90"/>
+      <c r="AA35" s="90"/>
+      <c r="AB35" s="90"/>
+      <c r="AI35" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBGBBGBBB'</v>
+      </c>
+    </row>
+    <row r="36" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I36" s="90"/>
+      <c r="J36" s="90"/>
+      <c r="K36" s="90"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="90"/>
+      <c r="N36" s="90"/>
+      <c r="O36" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P36" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q36" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R36" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S36" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T36" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U36" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="V36" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W36" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="X36" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y36" s="90"/>
+      <c r="Z36" s="90"/>
+      <c r="AA36" s="90"/>
+      <c r="AB36" s="90"/>
+      <c r="AI36" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBGGGGGGB'</v>
+      </c>
+    </row>
+    <row r="37" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I37" s="90"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="90"/>
+      <c r="L37" s="90"/>
+      <c r="M37" s="90"/>
+      <c r="N37" s="90"/>
+      <c r="O37" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="S37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="T37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="U37" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W37" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X37" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y37" s="90"/>
+      <c r="Z37" s="90"/>
+      <c r="AA37" s="90"/>
+      <c r="AB37" s="90"/>
+      <c r="AI37" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBBBBGBBB'</v>
+      </c>
+    </row>
+    <row r="38" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I38" s="90"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="90"/>
+      <c r="L38" s="90"/>
+      <c r="M38" s="90"/>
+      <c r="N38" s="90"/>
+      <c r="O38" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="R38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="S38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="T38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="U38" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="W38" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="X38" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y38" s="90"/>
+      <c r="Z38" s="90"/>
+      <c r="AA38" s="90"/>
+      <c r="AB38" s="90"/>
+      <c r="AI38" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBBBBGBBB'</v>
+      </c>
+    </row>
+    <row r="39" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="90"/>
+      <c r="M39" s="90"/>
+      <c r="N39" s="90"/>
+      <c r="O39" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="S39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="T39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="U39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="V39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="W39" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="X39" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y39" s="90"/>
+      <c r="Z39" s="90"/>
+      <c r="AA39" s="90"/>
+      <c r="AB39" s="90"/>
+      <c r="AI39" t="str">
+        <f t="shared" si="1"/>
+        <v>'BBBBBBBBBB'</v>
+      </c>
+    </row>
+    <row r="40" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="90"/>
+      <c r="N40" s="90"/>
+      <c r="O40" s="90"/>
+      <c r="P40" s="90"/>
+      <c r="Q40" s="90"/>
+      <c r="R40" s="90"/>
+      <c r="S40" s="90"/>
+      <c r="T40" s="90"/>
+      <c r="U40" s="90"/>
+      <c r="V40" s="90"/>
+      <c r="W40" s="90"/>
+      <c r="X40" s="90"/>
+      <c r="Y40" s="90"/>
+      <c r="Z40" s="90"/>
+      <c r="AA40" s="90"/>
+      <c r="AB40" s="90"/>
+    </row>
+    <row r="41" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I41" s="90"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="90"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="90"/>
+      <c r="N41" s="90"/>
+      <c r="O41" s="90"/>
+      <c r="P41" s="90"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="90"/>
+      <c r="S41" s="90"/>
+      <c r="T41" s="90"/>
+      <c r="U41" s="90"/>
+      <c r="V41" s="90"/>
+      <c r="W41" s="90"/>
+      <c r="X41" s="90"/>
+      <c r="Y41" s="90"/>
+      <c r="Z41" s="90"/>
+      <c r="AA41" s="90"/>
+      <c r="AB41" s="90"/>
+      <c r="AI41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I42" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="90"/>
+      <c r="N42" s="90"/>
+      <c r="O42" s="90"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="90"/>
+      <c r="R42" s="90"/>
+      <c r="S42" s="90"/>
+      <c r="T42" s="90"/>
+      <c r="U42" s="90"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
+      <c r="X42" s="90"/>
+      <c r="Y42" s="90"/>
+      <c r="Z42" s="90"/>
+      <c r="AA42" s="90"/>
+      <c r="AB42" s="90"/>
+      <c r="AI42" s="94" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ42" s="95">
+        <f>13*9</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="90"/>
+      <c r="N43" s="90"/>
+      <c r="O43" s="90"/>
+      <c r="P43" s="90"/>
+      <c r="Q43" s="90"/>
+      <c r="R43" s="90"/>
+      <c r="S43" s="90"/>
+      <c r="T43" s="90"/>
+      <c r="U43" s="90"/>
+      <c r="V43" s="90"/>
+      <c r="W43" s="90"/>
+      <c r="X43" s="90"/>
+      <c r="Y43" s="90"/>
+      <c r="Z43" s="90"/>
+      <c r="AA43" s="90"/>
+      <c r="AB43" s="90"/>
+    </row>
+    <row r="44" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="AI44">
+        <f>17*13</f>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="9:36" x14ac:dyDescent="0.3">
+      <c r="Z47" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="N50" s="54">
+        <v>0</v>
+      </c>
+      <c r="O50" s="54">
+        <f>+N50+1</f>
+        <v>1</v>
+      </c>
+      <c r="P50" s="54">
+        <f t="shared" ref="P50:AB50" si="2">+O50+1</f>
+        <v>2</v>
+      </c>
+      <c r="Q50" s="54">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R50" s="54">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="S50" s="54">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="T50" s="54">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="U50" s="54">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="V50" s="54">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="W50" s="54">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="X50" s="54">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="Y50" s="54">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="Z50" s="54">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="AA50" s="54">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="AB50" s="54">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M51" s="54">
+        <v>0</v>
+      </c>
+      <c r="N51" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O51" t="s">
+        <v>24</v>
+      </c>
+      <c r="P51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>24</v>
+      </c>
+      <c r="R51" t="s">
+        <v>24</v>
+      </c>
+      <c r="S51" t="s">
+        <v>24</v>
+      </c>
+      <c r="T51" t="s">
+        <v>24</v>
+      </c>
+      <c r="U51" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="V51" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="W51" s="102" t="s">
+        <v>25</v>
+      </c>
+      <c r="X51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y51" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z51" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M52" s="54">
+        <f>+M51+1</f>
+        <v>1</v>
+      </c>
+      <c r="N52" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O52" t="s">
+        <v>24</v>
+      </c>
+      <c r="P52" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>24</v>
+      </c>
+      <c r="R52" t="s">
+        <v>24</v>
+      </c>
+      <c r="S52" t="s">
+        <v>24</v>
+      </c>
+      <c r="T52" t="s">
+        <v>24</v>
+      </c>
+      <c r="U52" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V52" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W52" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X52" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y52" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z52" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M53" s="54">
+        <f t="shared" ref="M53:M64" si="3">+M52+1</f>
+        <v>2</v>
+      </c>
+      <c r="N53" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O53" t="s">
+        <v>24</v>
+      </c>
+      <c r="P53" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>24</v>
+      </c>
+      <c r="R53" t="s">
+        <v>24</v>
+      </c>
+      <c r="S53" t="s">
+        <v>24</v>
+      </c>
+      <c r="T53" t="s">
+        <v>24</v>
+      </c>
+      <c r="U53" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V53" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W53" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X53" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y53" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z53" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M54" s="54">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N54" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O54" t="s">
+        <v>24</v>
+      </c>
+      <c r="P54" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>24</v>
+      </c>
+      <c r="R54" t="s">
+        <v>24</v>
+      </c>
+      <c r="S54" t="s">
+        <v>24</v>
+      </c>
+      <c r="T54" t="s">
+        <v>24</v>
+      </c>
+      <c r="U54" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V54" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W54" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X54" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y54" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z54" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M55" s="54">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="N55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="P55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U55" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V55" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W55" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA55" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB55" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M56" s="54">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="N56" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O56" t="s">
+        <v>25</v>
+      </c>
+      <c r="P56" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q56" s="108" t="s">
+        <v>25</v>
+      </c>
+      <c r="R56" s="108" t="s">
+        <v>25</v>
+      </c>
+      <c r="S56" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="T56" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="U56" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="V56" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="W56" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="X56" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y56" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z56" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA56" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB56" s="107" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M57" s="54">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N57" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O57" t="s">
+        <v>24</v>
+      </c>
+      <c r="P57" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>24</v>
+      </c>
+      <c r="R57" t="s">
+        <v>24</v>
+      </c>
+      <c r="S57" t="s">
+        <v>24</v>
+      </c>
+      <c r="T57" t="s">
+        <v>24</v>
+      </c>
+      <c r="U57" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V57" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W57" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X57" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y57" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z57" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M58" s="54">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N58" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O58" t="s">
+        <v>24</v>
+      </c>
+      <c r="P58" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>24</v>
+      </c>
+      <c r="R58" t="s">
+        <v>24</v>
+      </c>
+      <c r="S58" t="s">
+        <v>24</v>
+      </c>
+      <c r="T58" t="s">
+        <v>24</v>
+      </c>
+      <c r="U58" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V58" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W58" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X58" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y58" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z58" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M59" s="54">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O59" t="s">
+        <v>25</v>
+      </c>
+      <c r="P59" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U59" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V59" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W59" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA59" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB59" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M60" s="54">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="N60" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O60" t="s">
+        <v>24</v>
+      </c>
+      <c r="P60" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>24</v>
+      </c>
+      <c r="R60" t="s">
+        <v>24</v>
+      </c>
+      <c r="S60" t="s">
+        <v>24</v>
+      </c>
+      <c r="T60" t="s">
+        <v>24</v>
+      </c>
+      <c r="U60" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V60" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W60" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X60" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y60" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z60" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M61" s="54">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="N61" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O61" t="s">
+        <v>24</v>
+      </c>
+      <c r="P61" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>24</v>
+      </c>
+      <c r="R61" t="s">
+        <v>24</v>
+      </c>
+      <c r="S61" t="s">
+        <v>24</v>
+      </c>
+      <c r="T61" t="s">
+        <v>24</v>
+      </c>
+      <c r="U61" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="V61" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="W61" s="103" t="s">
+        <v>25</v>
+      </c>
+      <c r="X61" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y61" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z61" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M62" s="54">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="N62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="P62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="V62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="X62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA62" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB62" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M63" s="54">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="P63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="V63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="X63" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA63" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB63" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M64" s="54">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="N64" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O64" t="s">
+        <v>24</v>
+      </c>
+      <c r="P64" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>24</v>
+      </c>
+      <c r="R64" t="s">
+        <v>24</v>
+      </c>
+      <c r="S64" t="s">
+        <v>24</v>
+      </c>
+      <c r="T64" t="s">
+        <v>24</v>
+      </c>
+      <c r="U64" t="s">
+        <v>25</v>
+      </c>
+      <c r="V64" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W64" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="X64" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y64" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z64" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="N66" s="54">
+        <v>0</v>
+      </c>
+      <c r="O66" s="54">
+        <f>+N66+1</f>
+        <v>1</v>
+      </c>
+      <c r="P66" s="54">
+        <f t="shared" ref="P66:AB66" si="4">+O66+1</f>
+        <v>2</v>
+      </c>
+      <c r="Q66" s="54">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="R66" s="54">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="S66" s="54">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="T66" s="54">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="U66" s="54">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="V66" s="54">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="W66" s="54">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="X66" s="54">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Y66" s="54">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="Z66" s="54">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="AA66" s="54">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="AB66" s="54">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M67" s="54">
+        <v>0</v>
+      </c>
+      <c r="N67" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O67" t="s">
+        <v>24</v>
+      </c>
+      <c r="P67" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>24</v>
+      </c>
+      <c r="R67" t="s">
+        <v>24</v>
+      </c>
+      <c r="S67" t="s">
+        <v>24</v>
+      </c>
+      <c r="T67" t="s">
+        <v>24</v>
+      </c>
+      <c r="U67" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="V67" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W67" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="X67" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y67" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z67" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M68" s="54">
+        <f>+M67+1</f>
+        <v>1</v>
+      </c>
+      <c r="N68" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O68" t="s">
+        <v>24</v>
+      </c>
+      <c r="P68" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>24</v>
+      </c>
+      <c r="R68" t="s">
+        <v>24</v>
+      </c>
+      <c r="S68" t="s">
+        <v>24</v>
+      </c>
+      <c r="T68" t="s">
+        <v>24</v>
+      </c>
+      <c r="U68" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="V68" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W68" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="X68" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y68" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z68" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M69" s="54">
+        <f t="shared" ref="M69:M80" si="5">+M68+1</f>
+        <v>2</v>
+      </c>
+      <c r="N69" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O69" t="s">
+        <v>24</v>
+      </c>
+      <c r="P69" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>24</v>
+      </c>
+      <c r="R69" t="s">
+        <v>24</v>
+      </c>
+      <c r="S69" t="s">
+        <v>24</v>
+      </c>
+      <c r="T69" t="s">
+        <v>24</v>
+      </c>
+      <c r="U69" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="V69" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W69" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="X69" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y69" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z69" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M70" s="54">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N70" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O70" t="s">
+        <v>24</v>
+      </c>
+      <c r="P70" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>24</v>
+      </c>
+      <c r="R70" t="s">
+        <v>24</v>
+      </c>
+      <c r="S70" t="s">
+        <v>24</v>
+      </c>
+      <c r="T70" t="s">
+        <v>24</v>
+      </c>
+      <c r="U70" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="V70" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="W70" s="102" t="s">
+        <v>25</v>
+      </c>
+      <c r="X70" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y70" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z70" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M71" s="54">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="P71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T71" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U71" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V71" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="W71" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="X71" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y71" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z71" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA71" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB71" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M72" s="54">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="N72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O72" t="s">
+        <v>25</v>
+      </c>
+      <c r="P72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U72" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V72" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W72" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y72" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA72" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB72" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M73" s="54">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N73" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O73" t="s">
+        <v>24</v>
+      </c>
+      <c r="P73" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>24</v>
+      </c>
+      <c r="R73" t="s">
+        <v>24</v>
+      </c>
+      <c r="S73" t="s">
+        <v>24</v>
+      </c>
+      <c r="T73" t="s">
+        <v>24</v>
+      </c>
+      <c r="U73" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V73" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W73" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X73" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y73" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z73" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M74" s="54">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N74" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O74" t="s">
+        <v>24</v>
+      </c>
+      <c r="P74" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>24</v>
+      </c>
+      <c r="R74" t="s">
+        <v>24</v>
+      </c>
+      <c r="S74" t="s">
+        <v>24</v>
+      </c>
+      <c r="T74" t="s">
+        <v>24</v>
+      </c>
+      <c r="U74" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V74" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W74" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X74" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y74" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z74" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M75" s="54">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="N75" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O75" t="s">
+        <v>25</v>
+      </c>
+      <c r="P75" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q75" s="108" t="s">
+        <v>25</v>
+      </c>
+      <c r="R75" s="108" t="s">
+        <v>25</v>
+      </c>
+      <c r="S75" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="T75" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="U75" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="V75" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="W75" s="110" t="s">
+        <v>25</v>
+      </c>
+      <c r="X75" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y75" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z75" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA75" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB75" s="107" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M76" s="54">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N76" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O76" t="s">
+        <v>24</v>
+      </c>
+      <c r="P76" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>24</v>
+      </c>
+      <c r="R76" t="s">
+        <v>24</v>
+      </c>
+      <c r="S76" t="s">
+        <v>24</v>
+      </c>
+      <c r="T76" t="s">
+        <v>24</v>
+      </c>
+      <c r="U76" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V76" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W76" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X76" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y76" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z76" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA76" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M77" s="54">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="N77" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O77" t="s">
+        <v>24</v>
+      </c>
+      <c r="P77" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>24</v>
+      </c>
+      <c r="R77" t="s">
+        <v>24</v>
+      </c>
+      <c r="S77" t="s">
+        <v>24</v>
+      </c>
+      <c r="T77" t="s">
+        <v>24</v>
+      </c>
+      <c r="U77" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V77" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W77" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X77" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y77" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z77" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M78" s="54">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="N78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="P78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U78" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V78" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W78" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA78" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB78" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M79" s="54">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="N79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="P79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="S79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="T79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="U79" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="V79" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="W79" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="X79" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA79" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB79" s="96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="13:28" x14ac:dyDescent="0.3">
+      <c r="M80" s="54">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="N80" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O80" t="s">
+        <v>24</v>
+      </c>
+      <c r="P80" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>24</v>
+      </c>
+      <c r="R80" t="s">
+        <v>24</v>
+      </c>
+      <c r="S80" t="s">
+        <v>24</v>
+      </c>
+      <c r="T80" t="s">
+        <v>24</v>
+      </c>
+      <c r="U80" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="V80" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="W80" s="103" t="s">
+        <v>25</v>
+      </c>
+      <c r="X80" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y80" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z80" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="O51:T54 O64:U64 O57:T58 O59:P59 O60:T61 X60:X61 AA60:AB61 X57:X58 X51:X54 AA51:AB54 AA57:AB58 AA64:AB64 X63:X64 O56">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",O51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O67:T70 O80:T80 O73:T74 O75 O76:T77 X76:X77 AA76:AB77 X73:X74 X67:X70 AA67:AB70 AA73:AB74 AA80:AB80 X79:X80 O72">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",O67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Emas Supercomputer- HackerRank Problem Solving Challenge done
</commit_message>
<xml_diff>
--- a/HackerRank/Problem Solving/Observations/Challenges Observations.xlsx
+++ b/HackerRank/Problem Solving/Observations/Challenges Observations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\GR\Software Development\Learning\HackerRank\Problem Solving\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B35EE1-61D2-4740-89A0-672FF8D91926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B8FDED-26CA-4C36-A4F9-446315DE8F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="807" activeTab="4" xr2:uid="{02547566-692A-4121-816D-BFBD3A86BC7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="807" activeTab="4" xr2:uid="{02547566-692A-4121-816D-BFBD3A86BC7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Queens Attack" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="39">
   <si>
     <t>If qPos</t>
   </si>
@@ -137,6 +137,27 @@
   <si>
     <t>5 x 9</t>
   </si>
+  <si>
+    <t>0,7</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t>13,7</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -180,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +343,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -828,16 +861,6 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -858,11 +881,166 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7766,10 +7944,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCDF995-7901-458F-928B-4A20B2B19B7F}">
-  <dimension ref="I3:AJ80"/>
+  <dimension ref="M3:AJ121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA74" sqref="AA74"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI13" sqref="B13:AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7903,7 +8081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:36" x14ac:dyDescent="0.3">
       <c r="P17" s="84" t="s">
         <v>24</v>
       </c>
@@ -7930,7 +8108,7 @@
         <v>'BGBBGBB'</v>
       </c>
     </row>
-    <row r="18" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="15:36" x14ac:dyDescent="0.3">
       <c r="P18" s="84" t="s">
         <v>24</v>
       </c>
@@ -7957,7 +8135,7 @@
         <v>'BBBBGBB'</v>
       </c>
     </row>
-    <row r="19" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="15:36" x14ac:dyDescent="0.3">
       <c r="P19" s="84" t="s">
         <v>24</v>
       </c>
@@ -7984,7 +8162,7 @@
         <v>'BBGGGGG'</v>
       </c>
     </row>
-    <row r="20" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="15:36" x14ac:dyDescent="0.3">
       <c r="P20" s="84" t="s">
         <v>24</v>
       </c>
@@ -8011,7 +8189,7 @@
         <v>'BBBBGBB'</v>
       </c>
     </row>
-    <row r="21" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="15:36" x14ac:dyDescent="0.3">
       <c r="P21" s="86" t="s">
         <v>24</v>
       </c>
@@ -8038,140 +8216,26 @@
         <v>'BBBBGBB'</v>
       </c>
     </row>
-    <row r="23" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="15:36" x14ac:dyDescent="0.3">
       <c r="AI23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="AI24" s="94" t="s">
+    <row r="24" spans="15:36" x14ac:dyDescent="0.3">
+      <c r="AI24" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="AJ24" s="95">
+      <c r="AJ24" s="91">
         <f>5*9</f>
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="90"/>
-      <c r="O25" s="90"/>
-      <c r="P25" s="90"/>
-      <c r="Q25" s="90"/>
-      <c r="R25" s="90"/>
-      <c r="S25" s="90"/>
-      <c r="T25" s="90"/>
-      <c r="U25" s="90"/>
-      <c r="V25" s="90"/>
-      <c r="W25" s="90"/>
-      <c r="X25" s="90"/>
-      <c r="Y25" s="90"/>
-      <c r="Z25" s="90"/>
-      <c r="AA25" s="90"/>
-      <c r="AB25" s="90"/>
-    </row>
-    <row r="26" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I26" s="90"/>
-      <c r="J26" s="90"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="M26" s="90"/>
-      <c r="N26" s="90"/>
-      <c r="O26" s="90"/>
-      <c r="P26" s="90"/>
-      <c r="Q26" s="90"/>
-      <c r="R26" s="90"/>
-      <c r="S26" s="90"/>
-      <c r="T26" s="90"/>
-      <c r="U26" s="90"/>
-      <c r="V26" s="90"/>
-      <c r="W26" s="90"/>
-      <c r="X26" s="90"/>
-      <c r="Y26" s="90"/>
-      <c r="Z26" s="90"/>
-      <c r="AA26" s="90"/>
-      <c r="AB26" s="90"/>
-    </row>
-    <row r="27" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="90"/>
-      <c r="O27" s="90"/>
-      <c r="P27" s="90"/>
-      <c r="Q27" s="90"/>
-      <c r="R27" s="90"/>
-      <c r="S27" s="90"/>
-      <c r="T27" s="90"/>
-      <c r="U27" s="90"/>
-      <c r="V27" s="90"/>
-      <c r="W27" s="90"/>
-      <c r="X27" s="90"/>
-      <c r="Y27" s="90"/>
-      <c r="Z27" s="90"/>
-      <c r="AA27" s="90"/>
-      <c r="AB27" s="90"/>
-    </row>
-    <row r="28" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="90"/>
-      <c r="Q28" s="90"/>
-      <c r="R28" s="90"/>
-      <c r="S28" s="90"/>
-      <c r="T28" s="90"/>
-      <c r="U28" s="90"/>
-      <c r="V28" s="90"/>
-      <c r="W28" s="90"/>
-      <c r="X28" s="90"/>
-      <c r="Y28" s="90"/>
-      <c r="Z28" s="90"/>
-      <c r="AA28" s="90"/>
-      <c r="AB28" s="90"/>
+    <row r="28" spans="15:36" x14ac:dyDescent="0.3">
       <c r="AI28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="90"/>
-      <c r="Q29" s="90"/>
-      <c r="R29" s="90"/>
-      <c r="S29" s="90"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="90"/>
-      <c r="V29" s="90"/>
-      <c r="W29" s="90"/>
-      <c r="X29" s="90"/>
-      <c r="Y29" s="90"/>
-      <c r="Z29" s="90"/>
-      <c r="AA29" s="90"/>
-      <c r="AB29" s="90"/>
-    </row>
-    <row r="30" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="90"/>
-      <c r="N30" s="90"/>
+    <row r="30" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O30" s="76" t="s">
         <v>24</v>
       </c>
@@ -8202,10 +8266,6 @@
       <c r="X30" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="Y30" s="90"/>
-      <c r="Z30" s="90"/>
-      <c r="AA30" s="90"/>
-      <c r="AB30" s="90"/>
       <c r="AI30" t="str">
         <f>+_xlfn.CONCAT("'",O30:X30,"'")</f>
         <v>'BBBGBBBBBB'</v>
@@ -8215,47 +8275,37 @@
         <v>['BBBGBBBBBB','BBBGBBBBBB','BBBGBBBBBB','GGGGGGGBBB','BBBGBBGBBB','BBBGBBGBBB','BBBGGGGGGB','BBBBBBGBBB','BBBBBBGBBB','BBBBBBBBBB']</v>
       </c>
     </row>
-    <row r="31" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I31" s="90"/>
-      <c r="J31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="90"/>
+    <row r="31" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O31" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P31" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q31" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R31" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="S31" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="T31" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="U31" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="V31" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W31" s="91" t="s">
+      <c r="P31" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q31" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R31" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S31" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T31" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U31" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V31" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W31" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X31" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y31" s="90"/>
-      <c r="Z31" s="90"/>
-      <c r="AA31" s="90"/>
-      <c r="AB31" s="90"/>
       <c r="AI31" t="str">
         <f t="shared" ref="AI31:AI39" si="1">+_xlfn.CONCAT("'",O31:X31,"'")</f>
         <v>'BBBGBBBBBB'</v>
@@ -8264,335 +8314,259 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I32" s="90"/>
-      <c r="J32" s="90"/>
-      <c r="K32" s="90"/>
-      <c r="L32" s="90"/>
-      <c r="M32" s="90"/>
-      <c r="N32" s="90"/>
+    <row r="32" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O32" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P32" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q32" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R32" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="S32" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="T32" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="U32" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="V32" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W32" s="91" t="s">
+      <c r="P32" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q32" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T32" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U32" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="V32" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W32" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X32" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y32" s="90"/>
-      <c r="Z32" s="90"/>
-      <c r="AA32" s="90"/>
-      <c r="AB32" s="90"/>
       <c r="AI32" t="str">
         <f t="shared" si="1"/>
         <v>'BBBGBBBBBB'</v>
       </c>
     </row>
-    <row r="33" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I33" s="90"/>
-      <c r="J33" s="90"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="90"/>
+    <row r="33" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O33" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="P33" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q33" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="R33" s="93" t="s">
-        <v>25</v>
-      </c>
-      <c r="S33" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="T33" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="U33" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="V33" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W33" s="91" t="s">
+      <c r="P33" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q33" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="R33" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="S33" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="T33" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="V33" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W33" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X33" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y33" s="90"/>
-      <c r="Z33" s="90"/>
-      <c r="AA33" s="90"/>
-      <c r="AB33" s="90"/>
       <c r="AI33" t="str">
         <f t="shared" si="1"/>
         <v>'GGGGGGGBBB'</v>
       </c>
     </row>
-    <row r="34" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="90"/>
+    <row r="34" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O34" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P34" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q34" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R34" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="S34" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="T34" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="U34" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="V34" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W34" s="91" t="s">
+      <c r="P34" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q34" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R34" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S34" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T34" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U34" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="V34" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W34" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X34" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y34" s="90"/>
-      <c r="Z34" s="90"/>
-      <c r="AA34" s="90"/>
-      <c r="AB34" s="90"/>
       <c r="AI34" t="str">
         <f t="shared" si="1"/>
         <v>'BBBGBBGBBB'</v>
       </c>
     </row>
-    <row r="35" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I35" s="90"/>
-      <c r="J35" s="90"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="90"/>
-      <c r="N35" s="90"/>
+    <row r="35" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O35" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P35" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q35" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R35" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="S35" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="T35" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="U35" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="V35" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W35" s="91" t="s">
+      <c r="P35" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q35" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R35" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S35" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T35" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U35" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="V35" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W35" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X35" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y35" s="90"/>
-      <c r="Z35" s="90"/>
-      <c r="AA35" s="90"/>
-      <c r="AB35" s="90"/>
       <c r="AI35" t="str">
         <f t="shared" si="1"/>
         <v>'BBBGBBGBBB'</v>
       </c>
     </row>
-    <row r="36" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I36" s="90"/>
-      <c r="J36" s="90"/>
-      <c r="K36" s="90"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="90"/>
-      <c r="N36" s="90"/>
+    <row r="36" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O36" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P36" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q36" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R36" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="S36" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="T36" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="U36" s="93" t="s">
-        <v>25</v>
-      </c>
-      <c r="V36" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="W36" s="92" t="s">
+      <c r="P36" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q36" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R36" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="S36" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="T36" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="U36" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="V36" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="W36" s="66" t="s">
         <v>25</v>
       </c>
       <c r="X36" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y36" s="90"/>
-      <c r="Z36" s="90"/>
-      <c r="AA36" s="90"/>
-      <c r="AB36" s="90"/>
       <c r="AI36" t="str">
         <f t="shared" si="1"/>
         <v>'BBBGGGGGGB'</v>
       </c>
     </row>
-    <row r="37" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I37" s="90"/>
-      <c r="J37" s="90"/>
-      <c r="K37" s="90"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="90"/>
-      <c r="N37" s="90"/>
+    <row r="37" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O37" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P37" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q37" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R37" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="S37" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="T37" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="U37" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="V37" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W37" s="91" t="s">
+      <c r="P37" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q37" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R37" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="S37" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T37" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U37" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="V37" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W37" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X37" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y37" s="90"/>
-      <c r="Z37" s="90"/>
-      <c r="AA37" s="90"/>
-      <c r="AB37" s="90"/>
       <c r="AI37" t="str">
         <f t="shared" si="1"/>
         <v>'BBBBBBGBBB'</v>
       </c>
     </row>
-    <row r="38" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I38" s="90"/>
-      <c r="J38" s="90"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="90"/>
-      <c r="N38" s="90"/>
+    <row r="38" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O38" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="P38" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q38" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="R38" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="S38" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="T38" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="U38" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="V38" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="W38" s="91" t="s">
+      <c r="P38" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q38" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="R38" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="S38" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="T38" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="U38" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="V38" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="W38" s="82" t="s">
         <v>24</v>
       </c>
       <c r="X38" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="Y38" s="90"/>
-      <c r="Z38" s="90"/>
-      <c r="AA38" s="90"/>
-      <c r="AB38" s="90"/>
       <c r="AI38" t="str">
         <f t="shared" si="1"/>
         <v>'BBBBBBGBBB'</v>
       </c>
     </row>
-    <row r="39" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I39" s="90"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="90"/>
-      <c r="L39" s="90"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="90"/>
+    <row r="39" spans="15:36" x14ac:dyDescent="0.3">
       <c r="O39" s="86" t="s">
         <v>24</v>
       </c>
@@ -8623,120 +8597,32 @@
       <c r="X39" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="Y39" s="90"/>
-      <c r="Z39" s="90"/>
-      <c r="AA39" s="90"/>
-      <c r="AB39" s="90"/>
       <c r="AI39" t="str">
         <f t="shared" si="1"/>
         <v>'BBBBBBBBBB'</v>
       </c>
     </row>
-    <row r="40" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I40" s="90"/>
-      <c r="J40" s="90"/>
-      <c r="K40" s="90"/>
-      <c r="L40" s="90"/>
-      <c r="M40" s="90"/>
-      <c r="N40" s="90"/>
-      <c r="O40" s="90"/>
-      <c r="P40" s="90"/>
-      <c r="Q40" s="90"/>
-      <c r="R40" s="90"/>
-      <c r="S40" s="90"/>
-      <c r="T40" s="90"/>
-      <c r="U40" s="90"/>
-      <c r="V40" s="90"/>
-      <c r="W40" s="90"/>
-      <c r="X40" s="90"/>
-      <c r="Y40" s="90"/>
-      <c r="Z40" s="90"/>
-      <c r="AA40" s="90"/>
-      <c r="AB40" s="90"/>
-    </row>
-    <row r="41" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I41" s="90"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="90"/>
-      <c r="N41" s="90"/>
-      <c r="O41" s="90"/>
-      <c r="P41" s="90"/>
-      <c r="Q41" s="90"/>
-      <c r="R41" s="90"/>
-      <c r="S41" s="90"/>
-      <c r="T41" s="90"/>
-      <c r="U41" s="90"/>
-      <c r="V41" s="90"/>
-      <c r="W41" s="90"/>
-      <c r="X41" s="90"/>
-      <c r="Y41" s="90"/>
-      <c r="Z41" s="90"/>
-      <c r="AA41" s="90"/>
-      <c r="AB41" s="90"/>
+    <row r="41" spans="15:36" x14ac:dyDescent="0.3">
       <c r="AI41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I42" s="90"/>
-      <c r="J42" s="90"/>
-      <c r="K42" s="90"/>
-      <c r="L42" s="90"/>
-      <c r="M42" s="90"/>
-      <c r="N42" s="90"/>
-      <c r="O42" s="90"/>
-      <c r="P42" s="90"/>
-      <c r="Q42" s="90"/>
-      <c r="R42" s="90"/>
-      <c r="S42" s="90"/>
-      <c r="T42" s="90"/>
-      <c r="U42" s="90"/>
-      <c r="V42" s="90"/>
-      <c r="W42" s="90"/>
-      <c r="X42" s="90"/>
-      <c r="Y42" s="90"/>
-      <c r="Z42" s="90"/>
-      <c r="AA42" s="90"/>
-      <c r="AB42" s="90"/>
-      <c r="AI42" s="94" t="s">
+    <row r="42" spans="15:36" x14ac:dyDescent="0.3">
+      <c r="AI42" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="AJ42" s="95">
+      <c r="AJ42" s="91">
         <f>13*9</f>
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="9:36" x14ac:dyDescent="0.3">
-      <c r="I43" s="90"/>
-      <c r="J43" s="90"/>
-      <c r="K43" s="90"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="90"/>
-      <c r="N43" s="90"/>
-      <c r="O43" s="90"/>
-      <c r="P43" s="90"/>
-      <c r="Q43" s="90"/>
-      <c r="R43" s="90"/>
-      <c r="S43" s="90"/>
-      <c r="T43" s="90"/>
-      <c r="U43" s="90"/>
-      <c r="V43" s="90"/>
-      <c r="W43" s="90"/>
-      <c r="X43" s="90"/>
-      <c r="Y43" s="90"/>
-      <c r="Z43" s="90"/>
-      <c r="AA43" s="90"/>
-      <c r="AB43" s="90"/>
-    </row>
-    <row r="44" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="15:36" x14ac:dyDescent="0.3">
       <c r="AI44">
         <f>17*13</f>
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="9:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="15:36" x14ac:dyDescent="0.3">
       <c r="Z47" s="26" t="s">
         <v>25</v>
       </c>
@@ -8806,7 +8692,7 @@
       <c r="M51" s="54">
         <v>0</v>
       </c>
-      <c r="N51" s="96" t="s">
+      <c r="N51" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O51" t="s">
@@ -8827,22 +8713,22 @@
       <c r="T51" t="s">
         <v>24</v>
       </c>
-      <c r="U51" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="V51" s="100" t="s">
-        <v>25</v>
-      </c>
-      <c r="W51" s="102" t="s">
+      <c r="U51" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="V51" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W51" s="98" t="s">
         <v>25</v>
       </c>
       <c r="X51" t="s">
         <v>24</v>
       </c>
-      <c r="Y51" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z51" s="96" t="s">
+      <c r="Y51" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z51" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA51" t="s">
@@ -8857,7 +8743,7 @@
         <f>+M51+1</f>
         <v>1</v>
       </c>
-      <c r="N52" s="96" t="s">
+      <c r="N52" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O52" t="s">
@@ -8878,22 +8764,22 @@
       <c r="T52" t="s">
         <v>24</v>
       </c>
-      <c r="U52" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V52" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W52" s="98" t="s">
+      <c r="U52" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V52" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W52" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X52" t="s">
         <v>24</v>
       </c>
-      <c r="Y52" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z52" s="96" t="s">
+      <c r="Y52" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z52" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA52" t="s">
@@ -8908,7 +8794,7 @@
         <f t="shared" ref="M53:M64" si="3">+M52+1</f>
         <v>2</v>
       </c>
-      <c r="N53" s="96" t="s">
+      <c r="N53" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O53" t="s">
@@ -8929,22 +8815,22 @@
       <c r="T53" t="s">
         <v>24</v>
       </c>
-      <c r="U53" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V53" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W53" s="98" t="s">
+      <c r="U53" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V53" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W53" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X53" t="s">
         <v>24</v>
       </c>
-      <c r="Y53" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z53" s="96" t="s">
+      <c r="Y53" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z53" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA53" t="s">
@@ -8959,7 +8845,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="N54" s="96" t="s">
+      <c r="N54" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O54" t="s">
@@ -8980,22 +8866,22 @@
       <c r="T54" t="s">
         <v>24</v>
       </c>
-      <c r="U54" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V54" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W54" s="98" t="s">
+      <c r="U54" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V54" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W54" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X54" t="s">
         <v>24</v>
       </c>
-      <c r="Y54" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z54" s="96" t="s">
+      <c r="Y54" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z54" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA54" t="s">
@@ -9010,49 +8896,49 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="N55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="O55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="P55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U55" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V55" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W55" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="X55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA55" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB55" s="96" t="s">
+      <c r="N55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="O55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="P55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U55" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V55" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W55" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="X55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA55" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB55" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9061,49 +8947,49 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="N56" s="96" t="s">
+      <c r="N56" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O56" t="s">
         <v>25</v>
       </c>
-      <c r="P56" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q56" s="108" t="s">
-        <v>25</v>
-      </c>
-      <c r="R56" s="108" t="s">
-        <v>25</v>
-      </c>
-      <c r="S56" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="T56" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="U56" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="V56" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="W56" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="X56" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y56" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z56" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA56" s="106" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB56" s="107" t="s">
+      <c r="P56" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q56" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="R56" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="S56" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="T56" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="U56" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="V56" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="W56" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="X56" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y56" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z56" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA56" s="102" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB56" s="103" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9112,7 +8998,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="N57" s="96" t="s">
+      <c r="N57" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O57" t="s">
@@ -9133,22 +9019,22 @@
       <c r="T57" t="s">
         <v>24</v>
       </c>
-      <c r="U57" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V57" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W57" s="98" t="s">
+      <c r="U57" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V57" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W57" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X57" t="s">
         <v>24</v>
       </c>
-      <c r="Y57" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z57" s="96" t="s">
+      <c r="Y57" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z57" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA57" t="s">
@@ -9163,7 +9049,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="N58" s="96" t="s">
+      <c r="N58" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O58" t="s">
@@ -9184,22 +9070,22 @@
       <c r="T58" t="s">
         <v>24</v>
       </c>
-      <c r="U58" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V58" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W58" s="98" t="s">
+      <c r="U58" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V58" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W58" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X58" t="s">
         <v>24</v>
       </c>
-      <c r="Y58" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z58" s="96" t="s">
+      <c r="Y58" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z58" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA58" t="s">
@@ -9214,7 +9100,7 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="N59" s="96" t="s">
+      <c r="N59" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O59" t="s">
@@ -9223,40 +9109,40 @@
       <c r="P59" t="s">
         <v>25</v>
       </c>
-      <c r="Q59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U59" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V59" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W59" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="X59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA59" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB59" s="96" t="s">
+      <c r="Q59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U59" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V59" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W59" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="X59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA59" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB59" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9265,7 +9151,7 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="N60" s="96" t="s">
+      <c r="N60" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O60" t="s">
@@ -9286,22 +9172,22 @@
       <c r="T60" t="s">
         <v>24</v>
       </c>
-      <c r="U60" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V60" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W60" s="98" t="s">
+      <c r="U60" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V60" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W60" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X60" t="s">
         <v>24</v>
       </c>
-      <c r="Y60" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z60" s="96" t="s">
+      <c r="Y60" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z60" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA60" t="s">
@@ -9316,7 +9202,7 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N61" s="96" t="s">
+      <c r="N61" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O61" t="s">
@@ -9337,22 +9223,22 @@
       <c r="T61" t="s">
         <v>24</v>
       </c>
-      <c r="U61" s="99" t="s">
-        <v>25</v>
-      </c>
-      <c r="V61" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="W61" s="103" t="s">
+      <c r="U61" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="V61" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="W61" s="99" t="s">
         <v>25</v>
       </c>
       <c r="X61" t="s">
         <v>24</v>
       </c>
-      <c r="Y61" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z61" s="96" t="s">
+      <c r="Y61" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z61" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA61" t="s">
@@ -9367,49 +9253,49 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="N62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="O62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="P62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="V62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="W62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="X62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA62" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB62" s="96" t="s">
+      <c r="N62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="O62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="P62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="X62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA62" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB62" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9418,49 +9304,49 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="N63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="O63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="P63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="V63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="W63" s="96" t="s">
+      <c r="N63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="O63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="P63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W63" s="92" t="s">
         <v>25</v>
       </c>
       <c r="X63" t="s">
         <v>25</v>
       </c>
-      <c r="Y63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA63" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB63" s="96" t="s">
+      <c r="Y63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA63" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB63" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9469,7 +9355,7 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="N64" s="96" t="s">
+      <c r="N64" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O64" t="s">
@@ -9493,19 +9379,19 @@
       <c r="U64" t="s">
         <v>25</v>
       </c>
-      <c r="V64" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="W64" s="96" t="s">
+      <c r="V64" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W64" s="92" t="s">
         <v>25</v>
       </c>
       <c r="X64" t="s">
         <v>24</v>
       </c>
-      <c r="Y64" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z64" s="96" t="s">
+      <c r="Y64" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z64" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA64" t="s">
@@ -9580,7 +9466,7 @@
       <c r="M67" s="54">
         <v>0</v>
       </c>
-      <c r="N67" s="96" t="s">
+      <c r="N67" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O67" t="s">
@@ -9601,22 +9487,22 @@
       <c r="T67" t="s">
         <v>24</v>
       </c>
-      <c r="U67" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="V67" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="W67" s="96" t="s">
+      <c r="U67" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V67" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W67" s="92" t="s">
         <v>25</v>
       </c>
       <c r="X67" t="s">
         <v>24</v>
       </c>
-      <c r="Y67" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z67" s="96" t="s">
+      <c r="Y67" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z67" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA67" t="s">
@@ -9631,7 +9517,7 @@
         <f>+M67+1</f>
         <v>1</v>
       </c>
-      <c r="N68" s="96" t="s">
+      <c r="N68" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O68" t="s">
@@ -9652,13 +9538,13 @@
       <c r="T68" t="s">
         <v>24</v>
       </c>
-      <c r="U68" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="V68" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="W68" s="96" t="s">
+      <c r="U68" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V68" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W68" s="92" t="s">
         <v>25</v>
       </c>
       <c r="X68" t="s">
@@ -9667,7 +9553,7 @@
       <c r="Y68" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z68" s="96" t="s">
+      <c r="Z68" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA68" t="s">
@@ -9682,7 +9568,7 @@
         <f t="shared" ref="M69:M80" si="5">+M68+1</f>
         <v>2</v>
       </c>
-      <c r="N69" s="96" t="s">
+      <c r="N69" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O69" t="s">
@@ -9703,13 +9589,13 @@
       <c r="T69" t="s">
         <v>24</v>
       </c>
-      <c r="U69" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="V69" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="W69" s="96" t="s">
+      <c r="U69" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="V69" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="W69" s="92" t="s">
         <v>25</v>
       </c>
       <c r="X69" t="s">
@@ -9718,7 +9604,7 @@
       <c r="Y69" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z69" s="96" t="s">
+      <c r="Z69" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA69" t="s">
@@ -9733,7 +9619,7 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="N70" s="96" t="s">
+      <c r="N70" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O70" t="s">
@@ -9754,13 +9640,13 @@
       <c r="T70" t="s">
         <v>24</v>
       </c>
-      <c r="U70" s="97" t="s">
-        <v>25</v>
-      </c>
-      <c r="V70" s="100" t="s">
-        <v>25</v>
-      </c>
-      <c r="W70" s="102" t="s">
+      <c r="U70" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="V70" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="W70" s="98" t="s">
         <v>25</v>
       </c>
       <c r="X70" t="s">
@@ -9769,7 +9655,7 @@
       <c r="Y70" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z70" s="96" t="s">
+      <c r="Z70" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA70" t="s">
@@ -9784,28 +9670,28 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="N71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="O71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="P71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T71" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U71" s="111" t="s">
+      <c r="N71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="O71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="P71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T71" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U71" s="107" t="s">
         <v>25</v>
       </c>
       <c r="V71" s="26" t="s">
@@ -9835,49 +9721,49 @@
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="N72" s="96" t="s">
+      <c r="N72" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O72" t="s">
         <v>25</v>
       </c>
-      <c r="P72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U72" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V72" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W72" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="X72" s="96" t="s">
+      <c r="P72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U72" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V72" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W72" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="X72" s="92" t="s">
         <v>25</v>
       </c>
       <c r="Y72" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA72" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB72" s="96" t="s">
+      <c r="Z72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA72" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB72" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9886,7 +9772,7 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="N73" s="96" t="s">
+      <c r="N73" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O73" t="s">
@@ -9907,13 +9793,13 @@
       <c r="T73" t="s">
         <v>24</v>
       </c>
-      <c r="U73" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V73" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W73" s="98" t="s">
+      <c r="U73" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V73" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W73" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X73" t="s">
@@ -9922,7 +9808,7 @@
       <c r="Y73" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z73" s="96" t="s">
+      <c r="Z73" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA73" t="s">
@@ -9937,7 +9823,7 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="N74" s="96" t="s">
+      <c r="N74" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O74" t="s">
@@ -9958,13 +9844,13 @@
       <c r="T74" t="s">
         <v>24</v>
       </c>
-      <c r="U74" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V74" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W74" s="98" t="s">
+      <c r="U74" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V74" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W74" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X74" t="s">
@@ -9973,7 +9859,7 @@
       <c r="Y74" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z74" s="96" t="s">
+      <c r="Z74" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA74" t="s">
@@ -9988,49 +9874,49 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="N75" s="96" t="s">
+      <c r="N75" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O75" t="s">
         <v>25</v>
       </c>
-      <c r="P75" s="104" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q75" s="108" t="s">
-        <v>25</v>
-      </c>
-      <c r="R75" s="108" t="s">
-        <v>25</v>
-      </c>
-      <c r="S75" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="T75" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="U75" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="V75" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="W75" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="X75" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y75" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z75" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA75" s="106" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB75" s="107" t="s">
+      <c r="P75" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q75" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="R75" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="S75" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="T75" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="U75" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="V75" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="W75" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="X75" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y75" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z75" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA75" s="102" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB75" s="103" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10039,7 +9925,7 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="N76" s="96" t="s">
+      <c r="N76" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O76" t="s">
@@ -10060,22 +9946,22 @@
       <c r="T76" t="s">
         <v>24</v>
       </c>
-      <c r="U76" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V76" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W76" s="98" t="s">
+      <c r="U76" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V76" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W76" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X76" t="s">
         <v>24</v>
       </c>
-      <c r="Y76" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z76" s="96" t="s">
+      <c r="Y76" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z76" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA76" t="s">
@@ -10090,7 +9976,7 @@
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="N77" s="96" t="s">
+      <c r="N77" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O77" t="s">
@@ -10111,22 +9997,22 @@
       <c r="T77" t="s">
         <v>24</v>
       </c>
-      <c r="U77" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V77" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W77" s="98" t="s">
+      <c r="U77" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V77" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W77" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X77" t="s">
         <v>24</v>
       </c>
-      <c r="Y77" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z77" s="96" t="s">
+      <c r="Y77" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z77" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA77" t="s">
@@ -10141,49 +10027,49 @@
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="N78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="O78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="P78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U78" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V78" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W78" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="X78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA78" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB78" s="96" t="s">
+      <c r="N78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="O78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="P78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U78" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V78" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W78" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="X78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA78" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB78" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10192,49 +10078,49 @@
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="N79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="O79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="P79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="R79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="S79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="T79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="U79" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="V79" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="W79" s="98" t="s">
+      <c r="N79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="O79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="P79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="R79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="S79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="T79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="U79" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="V79" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="W79" s="94" t="s">
         <v>25</v>
       </c>
       <c r="X79" t="s">
         <v>25</v>
       </c>
-      <c r="Y79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA79" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB79" s="96" t="s">
+      <c r="Y79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA79" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB79" s="92" t="s">
         <v>25</v>
       </c>
     </row>
@@ -10243,7 +10129,7 @@
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="N80" s="96" t="s">
+      <c r="N80" s="92" t="s">
         <v>25</v>
       </c>
       <c r="O80" t="s">
@@ -10264,22 +10150,22 @@
       <c r="T80" t="s">
         <v>24</v>
       </c>
-      <c r="U80" s="99" t="s">
-        <v>25</v>
-      </c>
-      <c r="V80" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="W80" s="103" t="s">
+      <c r="U80" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="V80" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="W80" s="99" t="s">
         <v>25</v>
       </c>
       <c r="X80" t="s">
         <v>24</v>
       </c>
-      <c r="Y80" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z80" s="96" t="s">
+      <c r="Y80" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z80" s="92" t="s">
         <v>25</v>
       </c>
       <c r="AA80" t="s">
@@ -10289,15 +10175,773 @@
         <v>24</v>
       </c>
     </row>
+    <row r="83" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AE83" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI83" s="108" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AE84" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI84" s="61"/>
+    </row>
+    <row r="85" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AE85" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI85" s="61"/>
+    </row>
+    <row r="86" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AB86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH86" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI86" s="61"/>
+    </row>
+    <row r="87" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AE87" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI87" s="61"/>
+    </row>
+    <row r="88" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AE88" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI88" s="61"/>
+    </row>
+    <row r="89" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AE89" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI89" s="108" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ89" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AI90" s="61"/>
+    </row>
+    <row r="91" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AC91" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI91" s="108" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="92" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AC92" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI92" s="61"/>
+    </row>
+    <row r="93" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AC93" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI93" s="61"/>
+    </row>
+    <row r="94" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AC94" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI94" s="61"/>
+    </row>
+    <row r="95" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="AC95" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI95" s="61"/>
+    </row>
+    <row r="96" spans="24:36" x14ac:dyDescent="0.3">
+      <c r="X96" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y96" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z96" s="104" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA96" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB96" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC96" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD96" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE96" s="106" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF96" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG96" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH96" s="101" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI96" s="61"/>
+    </row>
+    <row r="97" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="AC97" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI97" s="61"/>
+    </row>
+    <row r="98" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="AC98" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI98" s="61"/>
+    </row>
+    <row r="99" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="AC99" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI99" s="61"/>
+    </row>
+    <row r="100" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="AC100" s="107" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI100" s="61"/>
+    </row>
+    <row r="101" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="AC101" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI101" s="108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="U109" s="54">
+        <v>0</v>
+      </c>
+      <c r="V109" s="54">
+        <f>+U109+1</f>
+        <v>1</v>
+      </c>
+      <c r="W109" s="54">
+        <f t="shared" ref="W109" si="6">+V109+1</f>
+        <v>2</v>
+      </c>
+      <c r="X109" s="54">
+        <f t="shared" ref="X109" si="7">+W109+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y109" s="54">
+        <f t="shared" ref="Y109" si="8">+X109+1</f>
+        <v>4</v>
+      </c>
+      <c r="Z109" s="54">
+        <f t="shared" ref="Z109" si="9">+Y109+1</f>
+        <v>5</v>
+      </c>
+      <c r="AA109" s="54">
+        <f t="shared" ref="AA109" si="10">+Z109+1</f>
+        <v>6</v>
+      </c>
+      <c r="AB109" s="54">
+        <f t="shared" ref="AB109" si="11">+AA109+1</f>
+        <v>7</v>
+      </c>
+      <c r="AC109" s="54">
+        <f t="shared" ref="AC109" si="12">+AB109+1</f>
+        <v>8</v>
+      </c>
+      <c r="AD109" s="54">
+        <f t="shared" ref="AD109" si="13">+AC109+1</f>
+        <v>9</v>
+      </c>
+      <c r="AE109" s="54">
+        <f t="shared" ref="AE109" si="14">+AD109+1</f>
+        <v>10</v>
+      </c>
+      <c r="AF109" s="54">
+        <f t="shared" ref="AF109" si="15">+AE109+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="T110" s="54">
+        <v>0</v>
+      </c>
+      <c r="U110" s="109">
+        <v>0</v>
+      </c>
+      <c r="V110" s="109">
+        <v>0</v>
+      </c>
+      <c r="W110" s="109">
+        <v>0</v>
+      </c>
+      <c r="X110" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y110" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z110" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA110" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB110" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC110" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD110" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE110" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF110" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="T111" s="54">
+        <f>+T110+1</f>
+        <v>1</v>
+      </c>
+      <c r="U111" s="109">
+        <v>0</v>
+      </c>
+      <c r="V111" s="109">
+        <v>0</v>
+      </c>
+      <c r="W111" s="109">
+        <v>0</v>
+      </c>
+      <c r="X111" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y111" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z111" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA111" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB111" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC111" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD111" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE111" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF111" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="20:35" x14ac:dyDescent="0.3">
+      <c r="T112" s="54">
+        <f t="shared" ref="T112:T121" si="16">+T111+1</f>
+        <v>2</v>
+      </c>
+      <c r="U112" s="109">
+        <v>0</v>
+      </c>
+      <c r="V112" s="109">
+        <v>0</v>
+      </c>
+      <c r="W112" s="109">
+        <v>0</v>
+      </c>
+      <c r="X112" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y112" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z112" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA112" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB112" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC112" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD112" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE112" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF112" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T113" s="54">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="U113" s="109">
+        <v>0</v>
+      </c>
+      <c r="V113" s="109">
+        <v>0</v>
+      </c>
+      <c r="W113" s="109">
+        <v>0</v>
+      </c>
+      <c r="X113" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y113" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z113" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA113" s="110">
+        <v>0</v>
+      </c>
+      <c r="AB113" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC113" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD113" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE113" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF113" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T114" s="54">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="U114" s="109">
+        <v>0</v>
+      </c>
+      <c r="V114" s="109">
+        <v>0</v>
+      </c>
+      <c r="W114" s="109">
+        <v>0</v>
+      </c>
+      <c r="X114" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y114" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z114" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA114" s="110">
+        <v>0</v>
+      </c>
+      <c r="AB114" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC114" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD114" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE114" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF114" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T115" s="54">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="U115" s="109">
+        <v>0</v>
+      </c>
+      <c r="V115" s="109">
+        <v>0</v>
+      </c>
+      <c r="W115" s="109">
+        <v>0</v>
+      </c>
+      <c r="X115" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y115" s="110">
+        <v>0</v>
+      </c>
+      <c r="Z115" s="110">
+        <v>0</v>
+      </c>
+      <c r="AA115" s="110">
+        <v>0</v>
+      </c>
+      <c r="AB115" s="110">
+        <v>0</v>
+      </c>
+      <c r="AC115" s="112">
+        <v>0</v>
+      </c>
+      <c r="AD115" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE115" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF115" s="109">
+        <v>0</v>
+      </c>
+      <c r="AH115" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="116" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T116" s="54">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="U116" s="109">
+        <v>0</v>
+      </c>
+      <c r="V116" s="109">
+        <v>0</v>
+      </c>
+      <c r="W116" s="109">
+        <v>0</v>
+      </c>
+      <c r="X116" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y116" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z116" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA116" s="110">
+        <v>0</v>
+      </c>
+      <c r="AB116" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC116" s="111">
+        <v>0</v>
+      </c>
+      <c r="AD116" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE116" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF116" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T117" s="54">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="U117" s="109">
+        <v>0</v>
+      </c>
+      <c r="V117" s="109">
+        <v>0</v>
+      </c>
+      <c r="W117" s="109">
+        <v>0</v>
+      </c>
+      <c r="X117" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y117" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z117" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA117" s="112">
+        <v>0</v>
+      </c>
+      <c r="AB117" s="111">
+        <v>0</v>
+      </c>
+      <c r="AC117" s="111">
+        <v>0</v>
+      </c>
+      <c r="AD117" s="111">
+        <v>0</v>
+      </c>
+      <c r="AE117" s="111">
+        <v>0</v>
+      </c>
+      <c r="AF117" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T118" s="54">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="U118" s="109">
+        <v>0</v>
+      </c>
+      <c r="V118" s="109">
+        <v>0</v>
+      </c>
+      <c r="W118" s="109">
+        <v>0</v>
+      </c>
+      <c r="X118" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y118" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z118" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA118" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB118" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC118" s="111">
+        <v>0</v>
+      </c>
+      <c r="AD118" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE118" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF118" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T119" s="54">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="U119" s="109">
+        <v>0</v>
+      </c>
+      <c r="V119" s="109">
+        <v>0</v>
+      </c>
+      <c r="W119" s="109">
+        <v>0</v>
+      </c>
+      <c r="X119" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y119" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z119" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA119" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB119" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC119" s="111">
+        <v>0</v>
+      </c>
+      <c r="AD119" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE119" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF119" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T120" s="54">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="U120" s="109">
+        <v>0</v>
+      </c>
+      <c r="V120" s="109">
+        <v>0</v>
+      </c>
+      <c r="W120" s="109">
+        <v>0</v>
+      </c>
+      <c r="X120" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y120" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA120" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB120" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC120" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD120" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE120" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF120" s="109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="20:34" x14ac:dyDescent="0.3">
+      <c r="T121" s="54">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="U121" s="109">
+        <v>0</v>
+      </c>
+      <c r="V121" s="109">
+        <v>0</v>
+      </c>
+      <c r="W121" s="109">
+        <v>0</v>
+      </c>
+      <c r="X121" s="109">
+        <v>0</v>
+      </c>
+      <c r="Y121" s="109">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="109">
+        <v>0</v>
+      </c>
+      <c r="AA121" s="109">
+        <v>0</v>
+      </c>
+      <c r="AB121" s="109">
+        <v>0</v>
+      </c>
+      <c r="AC121" s="109">
+        <v>0</v>
+      </c>
+      <c r="AD121" s="109">
+        <v>0</v>
+      </c>
+      <c r="AE121" s="109">
+        <v>0</v>
+      </c>
+      <c r="AF121" s="109">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="O51:T54 O64:U64 O57:T58 O59:P59 O60:T61 X60:X61 AA60:AB61 X57:X58 X51:X54 AA51:AB54 AA57:AB58 AA64:AB64 X63:X64 O56">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="G">
+  <conditionalFormatting sqref="O51:T54 X51:X54 AA51:AB54 O56 O57:T58 X57:X58 AA57:AB58 O59:P59 O60:T61 X60:X61 AA60:AB61 X63:X64 O64:U64 AA64:AB64">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH("G",O51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O67:T70 O80:T80 O73:T74 O75 O76:T77 X76:X77 AA76:AB77 X73:X74 X67:X70 AA67:AB70 AA73:AB74 AA80:AB80 X79:X80 O72">
+  <conditionalFormatting sqref="O67:T70 X67:X70 AA67:AB70 O72 O73:T74 X73:X74 AA73:AB74 O75 O76:T77 X76:X77 AA76:AB77 X79:X80 O80:T80 AA80:AB80">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",O67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE110:AE112 V115 V120 AE120 U121:V121 X121 AE115:AE118 X119:Y120 W118:W121 U118:V119 Z110:AB112 Y118 AA118:AB118 AA119:AA120 V116:Z116 Z118:Z120 X115:Z115 Z113:Z114 AB113:AB115 AA115:AA116 U110:Y114 U117:AF117">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",U110)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB116">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",AB116)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA113">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",AA113)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD116">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",AD116)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD118:AD119">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="G">
+      <formula>NOT(ISERROR(SEARCH("G",AD118)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF115">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="G">
-      <formula>NOT(ISERROR(SEARCH("G",O67)))</formula>
+      <formula>NOT(ISERROR(SEARCH("G",AF115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>